<commit_message>
added empty demands sheet for Fill R comparison
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_MIG.xlsx
+++ b/SuppXLS/Scen_MIG.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\osemosys_India\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\py_projects\GitHub\osemosys_India\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8704205F-3006-4261-B02E-094DE46B66C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD9F555-D7FE-4730-BE82-E591A254285B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29190" yWindow="390" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="demands" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -398,7 +399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -480,4 +481,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D54CF8E-CB76-44AC-8683-9DD84E84923B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>